<commit_message>
Implement input validation, add generate QR button, and update UI
</commit_message>
<xml_diff>
--- a/public/qr_metadata.xlsx
+++ b/public/qr_metadata.xlsx
@@ -289,6 +289,15 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/pro-working-class-anti-war-Lowell-9ea3ef54ef63ade6af4ce930c103d363cd3c34ca1e43c84492dbb537d94c5569</t>
   </si>
   <si>
+    <t>Fish Pier</t>
+  </si>
+  <si>
+    <t>Fish Pier Commercial Seafood Small Trucks</t>
+  </si>
+  <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/pro-working-class-anti-war-Fish Pier-c87625d57c563b13450bcdb3fb0036181da9efb8cdb40cf4f62da2908e2d82a2</t>
+  </si>
+  <si>
     <t>Long Wharf Columbus Park</t>
   </si>
   <si>
@@ -298,15 +307,6 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/pro-working-class-anti-war-Long Wharf Columbus Park-3d82b1caa846ef949ea55d086086a4d080e05acc6b98ef41b02f6029d4d85f80</t>
   </si>
   <si>
-    <t>Fish Pier</t>
-  </si>
-  <si>
-    <t>Fish Pier Commercial Seafood Small Trucks</t>
-  </si>
-  <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/pro-working-class-anti-war-Fish Pier-c87625d57c563b13450bcdb3fb0036181da9efb8cdb40cf4f62da2908e2d82a2</t>
-  </si>
-  <si>
     <t>Revere Beach</t>
   </si>
   <si>
@@ -358,24 +358,24 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Orange Community College-6d5c0239fe5d91e883e09bbd20dfeeed71d414732a68bb68497e7ca2036082ac</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Lawrence-631c463744af845fc3659d213333290ddba445b0106c928ae6b1868107fcff4f</t>
+  </si>
+  <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Blue Maverick-aa5cd5bc19f57a3a07a1d0a04b2c9fc7ecc0538cee63a4d3eccc9f5d2262c6f3</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Green Boston University-0c179c47f88e3c531ee36d2d049972d4ba6bcc798588a27727c10133328993ac</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Blue Maverick-aa5cd5bc19f57a3a07a1d0a04b2c9fc7ecc0538cee63a4d3eccc9f5d2262c6f3</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Red Harvard-103a030258c3727af56e9092203caf48940fdba02faa3d24e45bb106b97c9317</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Lawrence-631c463744af845fc3659d213333290ddba445b0106c928ae6b1868107fcff4f</t>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Red Andrew-3621beb920ade34c010061c8f57972d8b269407ffdb17a22353704a8763fcc1c</t>
   </si>
   <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Orange Malden Center-d6c03f7209b54d53f388e1611a8eafdd5d8f95e2e6c0c934eb78e00e6c7cda62</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Red Andrew-3621beb920ade34c010061c8f57972d8b269407ffdb17a22353704a8763fcc1c</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Lynn-3bbc84812eed4689a1796b0ebbfb1b704706496fdc2b5a6b9db6705e8e78fcea</t>
   </si>
   <si>
@@ -385,51 +385,51 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Boston Wharfs-ce36e464e71cabd88f16065565d4cf6c61e96e7b57f9f98eee8df9fcd21db42e</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Blue Revere Beach-7476a70a55569b7dd9cce97de34f173229b1214069cc5e154f775fb5c90cbe4f</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-North Andover-4a58dd3ae384595dba9c4b5aaac65abef3acbc1a51fb0924358020ba7f1dcc58</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Blue Revere Beach-7476a70a55569b7dd9cce97de34f173229b1214069cc5e154f775fb5c90cbe4f</t>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Red JFK-b4ed4de91ba3d9ebd029e968d9b6e9feae4da1ab9561e2c3f91882863bbcab2b</t>
   </si>
   <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Wellesley College-89c75be5158ec161fa77f12bc81da9c168a4bfc7b59d0a00199e164c519d8ec8</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Red JFK-b4ed4de91ba3d9ebd029e968d9b6e9feae4da1ab9561e2c3f91882863bbcab2b</t>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Harvard Sq-597f1e609a12794dd9ce4476bd346602765264e3adf144ce38c235ddb4724bfa</t>
   </si>
   <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Revere-1208e3f80c6019e83549ff40f0e3a5d51e4628e3cd28e5e3751734216726170c</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Harvard Sq-597f1e609a12794dd9ce4476bd346602765264e3adf144ce38c235ddb4724bfa</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Red Ashmont-51d64b337fce70d97264428fc2899628f8d2f4a44212773d085a966fae197aa7</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Blue Airport-0a4c0aa4623adbab299e59b03649cb7a1f7a918aab958adb8f9303e1ad2d58a4</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Blue Wonderland-8802e35c7012b0a4ebe27abff1f1b09d93a3e8a030c4c795f3d63777ef54eeb0</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Blue Airport-0a4c0aa4623adbab299e59b03649cb7a1f7a918aab958adb8f9303e1ad2d58a4</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Orange Oak Grove-2727bcc80bfd3c8fbbc34244e5903f93631dc3316cde760418214184caaf965f</t>
   </si>
   <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Orange Ruggles-da491e6cbf22c9b420c87c99de092304e72b36cac2f012c6219f593cc061c0be</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Orange Forest Hills-ffc78e4c2d58335fe48267e323e805dbcd8ff2c65611ca687bf709d94019a7a0</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-UMass Boston-ef27a516f82983a8f5fd39bce5469e44ec82c34f9e719139f1ded64b14d1d3d8</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Orange Forest Hills-ffc78e4c2d58335fe48267e323e805dbcd8ff2c65611ca687bf709d94019a7a0</t>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Red Quincy Center-157cdbb998ba76364bc904d2b94d2c33e00295c5a73e7fa755dcb9413afff1be</t>
   </si>
   <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Battery Wharf-2227cf1723a292b7a3b8e61d5039c008b5d377a0fa4fee79772dc631cf251a0e</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Red Quincy Center-157cdbb998ba76364bc904d2b94d2c33e00295c5a73e7fa755dcb9413afff1be</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Green Boston College-5c58d99c0afc7fc80fb343163e18b53bdc89938d0b9c6a3ba0cd17908c76fc25</t>
   </si>
   <si>
@@ -442,12 +442,12 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Long Wharf Columbus Park-fbe349ba5b0b459f8488d5134ec67f0a55829560fa4fabb343990839f11ef333</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Revere Beach-3713f1adabaa9d052d73424bbcbcb06ba7b6f8d5db063bf3264735576a4acb08</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-New Bedford-46b204fe2f4bbdeccf91651eb52e66db6e33512acd14ade45f6ab020ab338ce9</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Revere Beach-3713f1adabaa9d052d73424bbcbcb06ba7b6f8d5db063bf3264735576a4acb08</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/rebel-girl-poster-Red Fields Corner-433dba1c5091a3c536cb1b3b045a8aff3236d97661ff93b42c9488d8d7246770</t>
   </si>
   <si>
@@ -478,12 +478,12 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Green Boston University-d017c00f17ffbb0fc8b1f990a843175867fc7566c0a191726976cd044e33bacd</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Red Andrew-9a623c6233364b4bd16c73aaad2510b822b3a2381385823683f6f92fc96d6e88</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Red Harvard-2266b6ac3bcc9a3448f6f2b1d08dad23a85c003a47cc2a7b498c1e3cfde5c617</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Red Andrew-9a623c6233364b4bd16c73aaad2510b822b3a2381385823683f6f92fc96d6e88</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Orange Malden Center-6ed6fc1e4dbfa96df38532dad23ba14bf203dc8e0a955a91db827d27254b0c9a</t>
   </si>
   <si>
@@ -511,15 +511,15 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Revere-b967786509b957f491888e01717f3bce1c38635ab4e13a9568f432857b00c9f0</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Harvard Sq-69bea1fdebca3ab1d02c5441be4dd9742baa1f932e12dbd34ba9c6025b294026</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Red Ashmont-806020afa30c29c5ec950739dcd4c2b2570dfcd3da3e5378c33fdf8d26b8978e</t>
   </si>
   <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Blue Airport-2cd633a1b2c45e46ffe5ce92cd8fe9d4ad21ce256a27a6cf050e87f4f179678c</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Harvard Sq-69bea1fdebca3ab1d02c5441be4dd9742baa1f932e12dbd34ba9c6025b294026</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Blue Wonderland-c7e89a98f905d487e8574efc83a43fa0d9bf5b6f59e8ebeaeb9ed2d1fe66b468</t>
   </si>
   <si>
@@ -538,24 +538,24 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Battery Wharf-0d8efce62faffaf769ae061f80f383113769fe7f223c9cd215bf5e94eb17a476</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Red Quincy Center-16bbc1f341695fd02e616f11449128b0a07f5b161a5034f92425adfeff0ee1f5</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Green Boston College-b7a1b2c958be2e77dd387fa597c01d63d635049a0fe995b7177f08e39cb5b271</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Red Quincy Center-16bbc1f341695fd02e616f11449128b0a07f5b161a5034f92425adfeff0ee1f5</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Lowell-1dcbe3e14effedaf16f912b30ca0eb7c5c9538e937c5b5503e9181984addc79c</t>
   </si>
   <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Fish Pier-8bedd54608004cbe9c5ddf211b1076ceecd4e4a7303f411b1777f919ba6073f2</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Long Wharf Columbus Park-0df1605675e02a99d2aaf83390659586d3648f8ac7b9da18c2885575f5fdeddb</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Revere Beach-7a945068c12548ca702d4f4085728ca7bcc25484a9c2ff724aea64ba538eee8a</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-Long Wharf Columbus Park-0df1605675e02a99d2aaf83390659586d3648f8ac7b9da18c2885575f5fdeddb</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/fight-back-poster-New Bedford-6068f766a19ef358238a6621e4d72938ceeece795544f0b1320bb94d736dd4dc</t>
   </si>
   <si>
@@ -586,12 +586,12 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Blue Maverick-516ffa9cc4ee03355272760c636061126b204f21da7831cbc42705a6f863cb49</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Red Harvard-4daec06fc17d8dd4cfb7966dfd92347d62273425d9142be840fffec33394c832</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Green Boston University-8f1c0bed38ec656fe08e420a817d903ff9447c5cf7cd29e6fcbd4bd64bb00c6e</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Red Harvard-4daec06fc17d8dd4cfb7966dfd92347d62273425d9142be840fffec33394c832</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Red Andrew-a902a25b65ec6812d233c58f77771599f7ee8098f775f63e23813b27c14bdada</t>
   </si>
   <si>
@@ -610,10 +610,13 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Blue Revere Beach-e912090aa4f671c5c60aa0cc02538267278730136357bb5f0087d0aa0f968162</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Wellesley College-4c510207e271af9e2d786038164e433121b7c29c5b8d9ddb4affe436044cf521</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-North Andover-649c783ac7f6ca1af69832ec9299a72ed023b45f29fd196202a5fe32e21d8115</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Wellesley College-4c510207e271af9e2d786038164e433121b7c29c5b8d9ddb4affe436044cf521</t>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Red JFK-73615e05f313a2d791ec05635dedc70a8d553164cb3f3b43549ba5d4bcc5f282</t>
   </si>
   <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Revere-c9906f1b177e0e3545045608ad5ec9c12ef755836a553605e692bd89f6e0b891</t>
@@ -625,27 +628,24 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Red Ashmont-abb846856fa769350f4450759d28151c24451d6cefecb75051178c7867e595d5</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Blue Airport-fe0246021316b62ca9aa4f3805b2ebb8de0a0998c19cbf4539723f7673cafc9f</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Blue Wonderland-9f499e1eaba6238312ae46290e9009e96628ac698d1d948de248e381d4e9bff4</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Red JFK-73615e05f313a2d791ec05635dedc70a8d553164cb3f3b43549ba5d4bcc5f282</t>
-  </si>
-  <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Blue Airport-fe0246021316b62ca9aa4f3805b2ebb8de0a0998c19cbf4539723f7673cafc9f</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Orange Oak Grove-e3bc3d73259d33b4634f7a3e5c103249d5aed4f025873f669fe61a94b32c9be7</t>
   </si>
   <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Orange Ruggles-9dec3ac4dba4d07c9e8ae26cd894ab2b3fdffd0e1bdc4b6c333b833cb14ba8c7</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Orange Forest Hills-0604cdac56dca6c538a9cbf4e3dd22916627533b98a1d02fbf19eecacb24e288</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-UMass Boston-beca2af34990500cf9ce2c9aa99f855308ca987cee38fd2eb9d86c8a21ce58dd</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Orange Forest Hills-0604cdac56dca6c538a9cbf4e3dd22916627533b98a1d02fbf19eecacb24e288</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/revolutionary-poster-Battery Wharf-452bde8cd6fbaf1af6fbc04d40a4e6fbe5963362e3150445c61bb81749a326e9</t>
   </si>
   <si>
@@ -706,18 +706,18 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/freedom-fighter-poster-Red Andrew-938dd2b37db375a58d00f764ecc1a22bb9029e42fd1b570b361e5017199956b8</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/freedom-fighter-poster-Orange Malden Center-c239278dbc6e398774ec2d317f007f975b6c135a39ab23c9d3a3cf5f18d82ca5</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/freedom-fighter-poster-Lynn-99447ae2da01b8762d78cecaf5bddd5fdbbaa3d4a8a3428dd2b885a1e8a63483</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/freedom-fighter-poster-Orange Malden Center-c239278dbc6e398774ec2d317f007f975b6c135a39ab23c9d3a3cf5f18d82ca5</t>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/freedom-fighter-poster-Fall River-21822810be59ddf979949655cbeffe6eef7158caeccc79f0105376f7d27efcab</t>
   </si>
   <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/freedom-fighter-poster-Boston Wharfs-c628c13400ba162e9bf2a344587483c72fb1c338453990b9f305ed557eccffc8</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/freedom-fighter-poster-Fall River-21822810be59ddf979949655cbeffe6eef7158caeccc79f0105376f7d27efcab</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/freedom-fighter-poster-Blue Revere Beach-a02655b3fe87af922d41eb62db8814d92a4287675d60686fe93c5f2c9006d3bc</t>
   </si>
   <si>
@@ -796,15 +796,15 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/free-the-world-poster-Orange Sullivan Sq-9b638f8db02680db6adf93cce57ae756bbdbb7980f04b1fe4f33326c25eb6321</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/free-the-world-poster-Lawrence-e267438f2d1bd7dc5ea6f3a7b9d8a2a99da58bb764b475ec2c4e21d3515aa135</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/free-the-world-poster-Dewey Sq South Station-658bbad279a7fdf1393064527c6faa7a5c8c08552773b006401390be4a46e237</t>
   </si>
   <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/free-the-world-poster-Orange Community College-1e114ec2c3d7712de66265600363f8ba46cfabe7199a6ef54461eb4b0e98f8fc</t>
   </si>
   <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/free-the-world-poster-Lawrence-e267438f2d1bd7dc5ea6f3a7b9d8a2a99da58bb764b475ec2c4e21d3515aa135</t>
-  </si>
-  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/free-the-world-poster-Blue Maverick-24dbd9f442eb882ab715ce2f52749b00c4d8f45bf8795b47a87cd171b1e87b56</t>
   </si>
   <si>
@@ -889,13 +889,13 @@
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/free-the-world-poster-Revere Beach-cb8979f3858c5b27a9850eef6a1b687a60e2fc54cae1f72b0bffd92d318d7e40</t>
   </si>
   <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/free-the-world-poster-Red Fields Corner-f1ba2cb243542fdff79df187a3382c962d52eb98c48a0b116d5ba340651b9af4</t>
+  </si>
+  <si>
+    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/free-the-world-poster-Red Alewife-6d7b61f126f2013191819f7184141b54ffeef31ea34460ea34238c01e58eefbd</t>
+  </si>
+  <si>
     <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/free-the-world-poster-New Bedford-05f32d52cf3a17dec2cc2ee44be3b37c5dd5af5060bbb85833f893ef9351a01b</t>
-  </si>
-  <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/free-the-world-poster-Red Fields Corner-f1ba2cb243542fdff79df187a3382c962d52eb98c48a0b116d5ba340651b9af4</t>
-  </si>
-  <si>
-    <t>https://qrcodeapplication-4ecfc40322a3.herokuapp.com/track/free-the-world-poster-Red Alewife-6d7b61f126f2013191819f7184141b54ffeef31ea34460ea34238c01e58eefbd</t>
   </si>
 </sst>
 </file>
@@ -1953,10 +1953,10 @@
         <v>111</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E40" t="s">
         <v>115</v>
@@ -1987,10 +1987,10 @@
         <v>111</v>
       </c>
       <c r="C42" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D42" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E42" t="s">
         <v>117</v>
@@ -2004,10 +2004,10 @@
         <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E43" t="s">
         <v>118</v>
@@ -2021,10 +2021,10 @@
         <v>111</v>
       </c>
       <c r="C44" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D44" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E44" t="s">
         <v>119</v>
@@ -2038,10 +2038,10 @@
         <v>111</v>
       </c>
       <c r="C45" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D45" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E45" t="s">
         <v>120</v>
@@ -2106,10 +2106,10 @@
         <v>111</v>
       </c>
       <c r="C49" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D49" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E49" t="s">
         <v>124</v>
@@ -2123,10 +2123,10 @@
         <v>111</v>
       </c>
       <c r="C50" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E50" t="s">
         <v>125</v>
@@ -2140,10 +2140,10 @@
         <v>111</v>
       </c>
       <c r="C51" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D51" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E51" t="s">
         <v>126</v>
@@ -2157,10 +2157,10 @@
         <v>111</v>
       </c>
       <c r="C52" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D52" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E52" t="s">
         <v>127</v>
@@ -2174,10 +2174,10 @@
         <v>111</v>
       </c>
       <c r="C53" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E53" t="s">
         <v>128</v>
@@ -2191,10 +2191,10 @@
         <v>111</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E54" t="s">
         <v>129</v>
@@ -2225,10 +2225,10 @@
         <v>111</v>
       </c>
       <c r="C56" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D56" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E56" t="s">
         <v>131</v>
@@ -2242,10 +2242,10 @@
         <v>111</v>
       </c>
       <c r="C57" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D57" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E57" t="s">
         <v>132</v>
@@ -2293,10 +2293,10 @@
         <v>111</v>
       </c>
       <c r="C60" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D60" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E60" t="s">
         <v>135</v>
@@ -2310,10 +2310,10 @@
         <v>111</v>
       </c>
       <c r="C61" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D61" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E61" t="s">
         <v>136</v>
@@ -2327,10 +2327,10 @@
         <v>111</v>
       </c>
       <c r="C62" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D62" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E62" t="s">
         <v>137</v>
@@ -2344,10 +2344,10 @@
         <v>111</v>
       </c>
       <c r="C63" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D63" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E63" t="s">
         <v>138</v>
@@ -2395,10 +2395,10 @@
         <v>111</v>
       </c>
       <c r="C66" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D66" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E66" t="s">
         <v>141</v>
@@ -2412,10 +2412,10 @@
         <v>111</v>
       </c>
       <c r="C67" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D67" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E67" t="s">
         <v>142</v>
@@ -2429,10 +2429,10 @@
         <v>111</v>
       </c>
       <c r="C68" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D68" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E68" t="s">
         <v>143</v>
@@ -2446,10 +2446,10 @@
         <v>111</v>
       </c>
       <c r="C69" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D69" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E69" t="s">
         <v>144</v>
@@ -2599,10 +2599,10 @@
         <v>148</v>
       </c>
       <c r="C78" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D78" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E78" t="s">
         <v>155</v>
@@ -2616,10 +2616,10 @@
         <v>148</v>
       </c>
       <c r="C79" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D79" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E79" t="s">
         <v>156</v>
@@ -2786,10 +2786,10 @@
         <v>148</v>
       </c>
       <c r="C89" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D89" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E89" t="s">
         <v>166</v>
@@ -2803,10 +2803,10 @@
         <v>148</v>
       </c>
       <c r="C90" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D90" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E90" t="s">
         <v>167</v>
@@ -2820,10 +2820,10 @@
         <v>148</v>
       </c>
       <c r="C91" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D91" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E91" t="s">
         <v>168</v>
@@ -2939,10 +2939,10 @@
         <v>148</v>
       </c>
       <c r="C98" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D98" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E98" t="s">
         <v>175</v>
@@ -2956,10 +2956,10 @@
         <v>148</v>
       </c>
       <c r="C99" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D99" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E99" t="s">
         <v>176</v>
@@ -2990,10 +2990,10 @@
         <v>148</v>
       </c>
       <c r="C101" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D101" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E101" t="s">
         <v>178</v>
@@ -3007,10 +3007,10 @@
         <v>148</v>
       </c>
       <c r="C102" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D102" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E102" t="s">
         <v>179</v>
@@ -3024,10 +3024,10 @@
         <v>148</v>
       </c>
       <c r="C103" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D103" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="E103" t="s">
         <v>180</v>
@@ -3177,10 +3177,10 @@
         <v>185</v>
       </c>
       <c r="C112" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D112" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E112" t="s">
         <v>191</v>
@@ -3194,10 +3194,10 @@
         <v>185</v>
       </c>
       <c r="C113" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D113" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E113" t="s">
         <v>192</v>
@@ -3313,10 +3313,10 @@
         <v>185</v>
       </c>
       <c r="C120" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D120" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E120" t="s">
         <v>199</v>
@@ -3330,10 +3330,10 @@
         <v>185</v>
       </c>
       <c r="C121" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D121" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E121" t="s">
         <v>200</v>
@@ -3347,10 +3347,10 @@
         <v>185</v>
       </c>
       <c r="C122" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D122" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E122" t="s">
         <v>201</v>
@@ -3364,10 +3364,10 @@
         <v>185</v>
       </c>
       <c r="C123" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D123" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E123" t="s">
         <v>202</v>
@@ -3381,10 +3381,10 @@
         <v>185</v>
       </c>
       <c r="C124" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D124" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E124" t="s">
         <v>203</v>
@@ -3398,10 +3398,10 @@
         <v>185</v>
       </c>
       <c r="C125" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D125" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E125" t="s">
         <v>204</v>
@@ -3415,10 +3415,10 @@
         <v>185</v>
       </c>
       <c r="C126" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D126" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E126" t="s">
         <v>205</v>
@@ -3432,10 +3432,10 @@
         <v>185</v>
       </c>
       <c r="C127" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D127" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E127" t="s">
         <v>206</v>
@@ -3483,10 +3483,10 @@
         <v>185</v>
       </c>
       <c r="C130" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D130" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E130" t="s">
         <v>209</v>
@@ -3500,10 +3500,10 @@
         <v>185</v>
       </c>
       <c r="C131" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D131" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E131" t="s">
         <v>210</v>
@@ -3585,10 +3585,10 @@
         <v>185</v>
       </c>
       <c r="C136" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D136" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E136" t="s">
         <v>215</v>
@@ -3602,10 +3602,10 @@
         <v>185</v>
       </c>
       <c r="C137" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D137" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E137" t="s">
         <v>216</v>
@@ -3823,10 +3823,10 @@
         <v>222</v>
       </c>
       <c r="C150" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D150" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E150" t="s">
         <v>231</v>
@@ -3840,10 +3840,10 @@
         <v>222</v>
       </c>
       <c r="C151" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D151" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E151" t="s">
         <v>232</v>
@@ -3857,10 +3857,10 @@
         <v>222</v>
       </c>
       <c r="C152" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D152" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E152" t="s">
         <v>233</v>
@@ -3874,10 +3874,10 @@
         <v>222</v>
       </c>
       <c r="C153" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D153" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E153" t="s">
         <v>234</v>
@@ -4180,10 +4180,10 @@
         <v>222</v>
       </c>
       <c r="C171" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D171" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E171" t="s">
         <v>252</v>
@@ -4197,10 +4197,10 @@
         <v>222</v>
       </c>
       <c r="C172" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D172" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E172" t="s">
         <v>253</v>
@@ -4299,10 +4299,10 @@
         <v>259</v>
       </c>
       <c r="C178" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D178" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E178" t="s">
         <v>261</v>
@@ -4316,10 +4316,10 @@
         <v>259</v>
       </c>
       <c r="C179" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D179" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E179" t="s">
         <v>262</v>
@@ -4333,10 +4333,10 @@
         <v>259</v>
       </c>
       <c r="C180" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D180" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E180" t="s">
         <v>263</v>
@@ -4775,10 +4775,10 @@
         <v>259</v>
       </c>
       <c r="C206" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D206" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E206" t="s">
         <v>289</v>
@@ -4792,10 +4792,10 @@
         <v>259</v>
       </c>
       <c r="C207" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D207" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E207" t="s">
         <v>290</v>
@@ -4826,10 +4826,10 @@
         <v>259</v>
       </c>
       <c r="C209" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D209" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E209" t="s">
         <v>292</v>
@@ -4843,10 +4843,10 @@
         <v>259</v>
       </c>
       <c r="C210" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D210" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E210" t="s">
         <v>293</v>
@@ -4860,10 +4860,10 @@
         <v>259</v>
       </c>
       <c r="C211" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D211" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E211" t="s">
         <v>294</v>

</xml_diff>